<commit_message>
Added Python POC poc
</commit_message>
<xml_diff>
--- a/algorithm/training_set.xlsx
+++ b/algorithm/training_set.xlsx
@@ -1,24 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shingiskaani/Documents/GitHub/ludusengine/algorithm/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d0358412\Downloads\ludusengine-master\algorithm\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9960" yWindow="440" windowWidth="38040" windowHeight="25300" tabRatio="500"/>
+    <workbookView xWindow="9960" yWindow="444" windowWidth="38040" windowHeight="25296" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Ruleset" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -27,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="165">
   <si>
     <t>Short name</t>
   </si>
@@ -519,13 +516,16 @@
   </si>
   <si>
     <t>Otherteampoints</t>
+  </si>
+  <si>
+    <t>Challenge_class</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -558,6 +558,13 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -581,7 +588,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -599,6 +606,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -610,6 +620,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -934,20 +947,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W70"/>
+  <dimension ref="A1:X70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M71" sqref="M71"/>
+      <selection pane="bottomLeft" activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="6" width="16.1640625" customWidth="1"/>
+    <col min="5" max="6" width="16.109375" customWidth="1"/>
     <col min="7" max="17" width="19" customWidth="1"/>
+    <col min="24" max="24" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="6" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:24" s="6" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>145</v>
       </c>
@@ -1017,8 +1031,11 @@
       <c r="W1" s="4" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" ht="26" x14ac:dyDescent="0.15">
+      <c r="X1" s="7" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>119</v>
       </c>
@@ -1049,8 +1066,11 @@
       <c r="V2" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:23" ht="26" x14ac:dyDescent="0.15">
+      <c r="X2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -1081,8 +1101,11 @@
       <c r="V3" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:23" ht="26" x14ac:dyDescent="0.15">
+      <c r="X3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1100,8 +1123,11 @@
       <c r="V4" s="3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="5" spans="1:23" ht="26" x14ac:dyDescent="0.15">
+      <c r="X4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -1119,8 +1145,11 @@
       <c r="V5" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="6" spans="1:23" ht="39" x14ac:dyDescent="0.15">
+      <c r="X5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>119</v>
       </c>
@@ -1143,8 +1172,11 @@
       <c r="V6" s="1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="7" spans="1:23" ht="39" x14ac:dyDescent="0.15">
+      <c r="X6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -1167,8 +1199,11 @@
       <c r="V7" s="1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="8" spans="1:23" ht="26" x14ac:dyDescent="0.15">
+      <c r="X7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1184,8 +1219,11 @@
         <v>90</v>
       </c>
       <c r="V8" s="1"/>
-    </row>
-    <row r="9" spans="1:23" ht="39" x14ac:dyDescent="0.15">
+      <c r="X8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
@@ -1208,8 +1246,11 @@
       <c r="V9" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="X9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -1228,8 +1269,11 @@
       <c r="U10" s="2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="11" spans="1:23" ht="39" x14ac:dyDescent="0.15">
+      <c r="X10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -1254,8 +1298,11 @@
       <c r="V11" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="12" spans="1:23" ht="26" x14ac:dyDescent="0.15">
+      <c r="X11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
@@ -1278,8 +1325,11 @@
       <c r="V12" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="13" spans="1:23" ht="39" x14ac:dyDescent="0.15">
+      <c r="X12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
@@ -1300,8 +1350,11 @@
         <v>74</v>
       </c>
       <c r="V13" s="3"/>
-    </row>
-    <row r="14" spans="1:23" ht="39" x14ac:dyDescent="0.15">
+      <c r="X13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>119</v>
       </c>
@@ -1322,8 +1375,11 @@
         <v>74</v>
       </c>
       <c r="V14" s="3"/>
-    </row>
-    <row r="15" spans="1:23" ht="39" x14ac:dyDescent="0.15">
+      <c r="X14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>143</v>
       </c>
@@ -1347,8 +1403,11 @@
       <c r="W15" s="3" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="16" spans="1:23" ht="39" x14ac:dyDescent="0.15">
+      <c r="X15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>119</v>
       </c>
@@ -1371,8 +1430,11 @@
       <c r="V16" s="3" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="17" spans="1:23" ht="39" x14ac:dyDescent="0.15">
+      <c r="X16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>143</v>
       </c>
@@ -1398,8 +1460,11 @@
       <c r="W17" s="3" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="18" spans="1:23" ht="39" x14ac:dyDescent="0.15">
+      <c r="X17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>119</v>
       </c>
@@ -1424,8 +1489,11 @@
       <c r="V18" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="19" spans="1:23" ht="39" x14ac:dyDescent="0.15">
+      <c r="X18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>143</v>
       </c>
@@ -1453,8 +1521,11 @@
       <c r="W19" s="3" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="20" spans="1:23" ht="39" x14ac:dyDescent="0.15">
+      <c r="X19">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>7</v>
       </c>
@@ -1479,8 +1550,11 @@
       <c r="V20" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="21" spans="1:23" ht="52" x14ac:dyDescent="0.15">
+      <c r="X20">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>7</v>
       </c>
@@ -1508,8 +1582,11 @@
       <c r="V21" s="3" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="22" spans="1:23" ht="39" x14ac:dyDescent="0.15">
+      <c r="X21">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>7</v>
       </c>
@@ -1530,8 +1607,11 @@
         <v>72</v>
       </c>
       <c r="V22" s="3"/>
-    </row>
-    <row r="23" spans="1:23" ht="26" x14ac:dyDescent="0.15">
+      <c r="X22">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>7</v>
       </c>
@@ -1554,8 +1634,11 @@
       <c r="V23" s="3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="24" spans="1:23" ht="26" x14ac:dyDescent="0.15">
+      <c r="X23">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>119</v>
       </c>
@@ -1583,8 +1666,11 @@
       <c r="V24" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="25" spans="1:23" ht="39" x14ac:dyDescent="0.15">
+      <c r="X24">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>7</v>
       </c>
@@ -1612,8 +1698,11 @@
       <c r="V25" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="26" spans="1:23" ht="26" x14ac:dyDescent="0.15">
+      <c r="X25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>7</v>
       </c>
@@ -1636,8 +1725,11 @@
       <c r="V26" s="3" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="27" spans="1:23" ht="39" x14ac:dyDescent="0.15">
+      <c r="X26">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>8</v>
       </c>
@@ -1653,8 +1745,11 @@
         <v>53</v>
       </c>
       <c r="V27" s="3"/>
-    </row>
-    <row r="28" spans="1:23" ht="26" x14ac:dyDescent="0.15">
+      <c r="X27">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>8</v>
       </c>
@@ -1680,8 +1775,11 @@
         <v>35</v>
       </c>
       <c r="V28" s="3"/>
-    </row>
-    <row r="29" spans="1:23" ht="26" x14ac:dyDescent="0.15">
+      <c r="X28">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>7</v>
       </c>
@@ -1707,8 +1805,11 @@
         <v>35</v>
       </c>
       <c r="V29" s="3"/>
-    </row>
-    <row r="30" spans="1:23" ht="52" x14ac:dyDescent="0.15">
+      <c r="X29">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" ht="66" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>119</v>
       </c>
@@ -1731,8 +1832,11 @@
       <c r="V30" s="3" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="31" spans="1:23" ht="52" x14ac:dyDescent="0.15">
+      <c r="X30">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" ht="66" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>143</v>
       </c>
@@ -1758,8 +1862,11 @@
       <c r="W31" s="3" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="32" spans="1:23" ht="52" x14ac:dyDescent="0.15">
+      <c r="X31">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" ht="66" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>7</v>
       </c>
@@ -1782,8 +1889,11 @@
       <c r="V32" s="3" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="33" spans="1:23" ht="39" x14ac:dyDescent="0.15">
+      <c r="X32">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>119</v>
       </c>
@@ -1811,8 +1921,11 @@
       <c r="V33" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="34" spans="1:23" ht="39" x14ac:dyDescent="0.15">
+      <c r="X33">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>143</v>
       </c>
@@ -1843,8 +1956,11 @@
       <c r="W34" s="3" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="35" spans="1:23" ht="39" x14ac:dyDescent="0.15">
+      <c r="X34">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>7</v>
       </c>
@@ -1872,8 +1988,11 @@
       <c r="V35" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="36" spans="1:23" ht="26" x14ac:dyDescent="0.15">
+      <c r="X35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>8</v>
       </c>
@@ -1888,8 +2007,11 @@
         <v>27</v>
       </c>
       <c r="V36" s="3"/>
-    </row>
-    <row r="37" spans="1:23" ht="52" x14ac:dyDescent="0.15">
+      <c r="X36">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>8</v>
       </c>
@@ -1902,8 +2024,11 @@
       <c r="U37" s="3" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="38" spans="1:23" ht="39" x14ac:dyDescent="0.15">
+      <c r="X37">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>142</v>
       </c>
@@ -1931,8 +2056,11 @@
       <c r="V38" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="39" spans="1:23" ht="39" x14ac:dyDescent="0.15">
+      <c r="X38">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:24" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>8</v>
       </c>
@@ -1960,8 +2088,11 @@
       <c r="V39" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="40" spans="1:23" ht="39" x14ac:dyDescent="0.15">
+      <c r="X39">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:24" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>119</v>
       </c>
@@ -1989,8 +2120,11 @@
       <c r="V40" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="41" spans="1:23" ht="39" x14ac:dyDescent="0.15">
+      <c r="X40">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:24" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>143</v>
       </c>
@@ -2021,8 +2155,11 @@
       <c r="W41" s="3" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="42" spans="1:23" ht="39" x14ac:dyDescent="0.15">
+      <c r="X41">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:24" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>7</v>
       </c>
@@ -2050,8 +2187,11 @@
       <c r="V42" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="43" spans="1:23" ht="39" x14ac:dyDescent="0.15">
+      <c r="X42">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:24" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>142</v>
       </c>
@@ -2077,8 +2217,11 @@
       <c r="W43" s="3" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="44" spans="1:23" ht="39" x14ac:dyDescent="0.15">
+      <c r="X43">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:24" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>8</v>
       </c>
@@ -2102,8 +2245,11 @@
         <v>22</v>
       </c>
       <c r="V44" s="3"/>
-    </row>
-    <row r="45" spans="1:23" ht="52" x14ac:dyDescent="0.15">
+      <c r="X44">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="1:24" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>8</v>
       </c>
@@ -2126,8 +2272,11 @@
       <c r="V45" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="46" spans="1:23" ht="52" x14ac:dyDescent="0.15">
+      <c r="X45">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="46" spans="1:24" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>119</v>
       </c>
@@ -2150,8 +2299,11 @@
       <c r="V46" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="47" spans="1:23" ht="52" x14ac:dyDescent="0.15">
+      <c r="X46">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="47" spans="1:24" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>143</v>
       </c>
@@ -2177,8 +2329,11 @@
       <c r="W47" s="3" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="48" spans="1:23" ht="52" x14ac:dyDescent="0.15">
+      <c r="X47">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="48" spans="1:24" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>7</v>
       </c>
@@ -2201,8 +2356,11 @@
       <c r="V48" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="49" spans="1:23" ht="26" x14ac:dyDescent="0.15">
+      <c r="X48">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="49" spans="1:24" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>8</v>
       </c>
@@ -2220,8 +2378,11 @@
       <c r="V49" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="50" spans="1:23" ht="26" x14ac:dyDescent="0.15">
+      <c r="X49">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="50" spans="1:24" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>7</v>
       </c>
@@ -2247,8 +2408,11 @@
       <c r="V50" s="3" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="51" spans="1:23" ht="52" x14ac:dyDescent="0.15">
+      <c r="X50">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="51" spans="1:24" ht="66" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>142</v>
       </c>
@@ -2277,8 +2441,11 @@
       <c r="W51" s="3" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="52" spans="1:23" ht="52" x14ac:dyDescent="0.15">
+      <c r="X51">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="52" spans="1:24" ht="66" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>143</v>
       </c>
@@ -2307,8 +2474,11 @@
       <c r="W52" s="3" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="53" spans="1:23" ht="52" x14ac:dyDescent="0.15">
+      <c r="X52">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="53" spans="1:24" ht="66" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>7</v>
       </c>
@@ -2334,8 +2504,11 @@
         <v>118</v>
       </c>
       <c r="V53" s="3"/>
-    </row>
-    <row r="54" spans="1:23" ht="26" x14ac:dyDescent="0.15">
+      <c r="X53">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="54" spans="1:24" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>8</v>
       </c>
@@ -2363,8 +2536,11 @@
       <c r="V54" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="55" spans="1:23" ht="26" x14ac:dyDescent="0.15">
+      <c r="X54">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="55" spans="1:24" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>7</v>
       </c>
@@ -2392,8 +2568,11 @@
       <c r="V55" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="56" spans="1:23" ht="26" x14ac:dyDescent="0.15">
+      <c r="X55">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="56" spans="1:24" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>8</v>
       </c>
@@ -2421,8 +2600,11 @@
       <c r="V56" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="57" spans="1:23" ht="26" x14ac:dyDescent="0.15">
+      <c r="X56">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="57" spans="1:24" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>119</v>
       </c>
@@ -2443,8 +2625,11 @@
         <v>126</v>
       </c>
       <c r="V57" s="3"/>
-    </row>
-    <row r="58" spans="1:23" ht="39" x14ac:dyDescent="0.15">
+      <c r="X57">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="58" spans="1:24" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>8</v>
       </c>
@@ -2459,8 +2644,11 @@
         <v>95</v>
       </c>
       <c r="V58" s="3"/>
-    </row>
-    <row r="59" spans="1:23" ht="39" x14ac:dyDescent="0.15">
+      <c r="X58">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="59" spans="1:24" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>8</v>
       </c>
@@ -2481,8 +2669,11 @@
         <v>86</v>
       </c>
       <c r="V59" s="3"/>
-    </row>
-    <row r="60" spans="1:23" ht="39" x14ac:dyDescent="0.15">
+      <c r="X59">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="60" spans="1:24" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>7</v>
       </c>
@@ -2503,8 +2694,11 @@
         <v>86</v>
       </c>
       <c r="V60" s="3"/>
-    </row>
-    <row r="61" spans="1:23" ht="52" x14ac:dyDescent="0.15">
+      <c r="X60">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="61" spans="1:24" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>142</v>
       </c>
@@ -2533,8 +2727,11 @@
       <c r="W61" s="3" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="62" spans="1:23" ht="52" x14ac:dyDescent="0.15">
+      <c r="X61">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="62" spans="1:24" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>143</v>
       </c>
@@ -2563,8 +2760,11 @@
       <c r="W62" s="3" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="63" spans="1:23" ht="52" x14ac:dyDescent="0.15">
+      <c r="X62">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="63" spans="1:24" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>7</v>
       </c>
@@ -2590,8 +2790,11 @@
         <v>114</v>
       </c>
       <c r="V63" s="3"/>
-    </row>
-    <row r="64" spans="1:23" ht="26" x14ac:dyDescent="0.15">
+      <c r="X63">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="64" spans="1:24" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>142</v>
       </c>
@@ -2610,8 +2813,11 @@
       <c r="W64" s="3" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="65" spans="1:23" ht="39" x14ac:dyDescent="0.15">
+      <c r="X64">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="65" spans="1:24" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>143</v>
       </c>
@@ -2635,8 +2841,11 @@
       <c r="W65" s="3" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="66" spans="1:23" ht="39" x14ac:dyDescent="0.15">
+      <c r="X65">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="66" spans="1:24" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>143</v>
       </c>
@@ -2660,8 +2869,11 @@
       <c r="W66" s="3" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="67" spans="1:23" ht="39" x14ac:dyDescent="0.15">
+      <c r="X66">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="67" spans="1:24" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>8</v>
       </c>
@@ -2682,8 +2894,11 @@
         <v>77</v>
       </c>
       <c r="V67" s="3"/>
-    </row>
-    <row r="68" spans="1:23" ht="39" x14ac:dyDescent="0.15">
+      <c r="X67">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="68" spans="1:24" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>119</v>
       </c>
@@ -2704,8 +2919,11 @@
         <v>77</v>
       </c>
       <c r="V68" s="3"/>
-    </row>
-    <row r="69" spans="1:23" ht="39" x14ac:dyDescent="0.15">
+      <c r="X68">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="69" spans="1:24" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>142</v>
       </c>
@@ -2726,8 +2944,11 @@
         <v>74</v>
       </c>
       <c r="V69" s="3"/>
-    </row>
-    <row r="70" spans="1:23" ht="39" x14ac:dyDescent="0.15">
+      <c r="X69">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="70" spans="1:24" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>142</v>
       </c>
@@ -2749,6 +2970,9 @@
       </c>
       <c r="V70" s="3" t="s">
         <v>121</v>
+      </c>
+      <c r="X70">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -2757,7 +2981,7 @@
     <sortCondition ref="A2:A70"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>